<commit_message>
Limit purchase grant until 2030 for EVs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Grant_EVs.xlsx
+++ b/SuppXLS/Scen_TRA_Grant_EVs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9BBA7-635A-4127-B5E2-EB2FDBEF954E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680D018A-C7DF-490C-A58F-607E02583697}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Year</t>
   </si>
@@ -1689,10 +1689,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,7 +1700,7 @@
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -1762,7 +1762,9 @@
       <c r="D6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="14">
+        <v>2018</v>
+      </c>
       <c r="F6" s="15">
         <v>-5</v>
       </c>
@@ -1771,6 +1773,40 @@
         <v>70</v>
       </c>
       <c r="I6" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7">
+        <v>2025</v>
+      </c>
+      <c r="F7" s="15">
+        <v>-5</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>2030</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify purchase grant for PHEVs until 2030
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Grant_EVs.xlsx
+++ b/SuppXLS/Scen_TRA_Grant_EVs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680D018A-C7DF-490C-A58F-607E02583697}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE554C92-2442-48F4-9D7F-4979914BBD68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>Year</t>
   </si>
@@ -305,13 +305,16 @@
     </r>
   </si>
   <si>
+    <t>INVCOST</t>
+  </si>
+  <si>
+    <t>*New</t>
+  </si>
+  <si>
     <t>T-CAR-BEV*</t>
   </si>
   <si>
-    <t>INVCOST</t>
-  </si>
-  <si>
-    <t>*New</t>
+    <t>T-CAR-PHEV*</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -482,6 +485,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1689,10 +1695,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1703,7 +1709,7 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="34" width="10.6640625" customWidth="1"/>
     <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
@@ -1760,7 +1766,7 @@
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="14">
         <v>2018</v>
@@ -1770,15 +1776,15 @@
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D7" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7">
         <v>2025</v>
@@ -1787,27 +1793,81 @@
         <v>-5</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8">
         <v>2030</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="16">
         <v>0</v>
       </c>
       <c r="H8" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>72</v>
+      <c r="E9" s="14">
+        <v>2018</v>
+      </c>
+      <c r="F9" s="15">
+        <v>-5</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F10" s="15">
+        <v>-5</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="14">
+        <v>2030</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update purchase grant for EVs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Grant_EVs.xlsx
+++ b/SuppXLS/Scen_TRA_Grant_EVs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE554C92-2442-48F4-9D7F-4979914BBD68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88036A4A-4307-443A-A600-22CECA6C2FB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2532" yWindow="2100" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Year</t>
   </si>
@@ -311,10 +311,7 @@
     <t>*New</t>
   </si>
   <si>
-    <t>T-CAR-BEV*</t>
-  </si>
-  <si>
-    <t>T-CAR-PHEV*</t>
+    <t>T-CAR-BEV*,T-CAR-PHEV*</t>
   </si>
 </sst>
 </file>
@@ -487,7 +484,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1695,10 +1692,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,7 +1706,7 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="34" width="10.6640625" customWidth="1"/>
     <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
@@ -1786,12 +1783,13 @@
       <c r="D7" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E7">
-        <v>2025</v>
+      <c r="E7" s="14">
+        <v>2030</v>
       </c>
       <c r="F7" s="15">
         <v>-5</v>
       </c>
+      <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
         <v>72</v>
       </c>
@@ -1804,69 +1802,15 @@
         <v>70</v>
       </c>
       <c r="E8">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="F8" s="16">
-        <v>0</v>
+        <v>-1E-10</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>72</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="14">
-        <v>2018</v>
-      </c>
-      <c r="F9" s="15">
-        <v>-5</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="14">
-        <v>2025</v>
-      </c>
-      <c r="F10" s="15">
-        <v>-5</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="14">
-        <v>2030</v>
-      </c>
-      <c r="F11" s="16">
-        <v>0</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="14" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add INVCOST for 2035 in SUBRES and modify grant purchase year
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Grant_EVs.xlsx
+++ b/SuppXLS/Scen_TRA_Grant_EVs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88036A4A-4307-443A-A600-22CECA6C2FB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E55E89-2D7C-4EE9-94A4-6FDF2FAAE9FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2532" yWindow="2100" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,10 +1802,10 @@
         <v>70</v>
       </c>
       <c r="E8">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="F8" s="16">
-        <v>-1E-10</v>
+        <v>-1.0000000000000001E-5</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>72</v>

</xml_diff>